<commit_message>
Updated data.xlsx file dates
</commit_message>
<xml_diff>
--- a/backend/data.xlsx
+++ b/backend/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raji Roy\Desktop\CRM Project\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31053C73-065D-4C2E-8126-5F54B1A7E225}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DC465D-8CBF-4D12-A822-66DBCE2C0A87}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="22">
   <si>
     <t>id</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>Lost</t>
-  </si>
-  <si>
-    <t>0/0/0000</t>
   </si>
 </sst>
 </file>
@@ -966,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="F101" sqref="F101"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101:E150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3293,12 +3290,8 @@
         <f>VLOOKUP(B101,team!A:B,2,FALSE)</f>
         <v>Belle</v>
       </c>
-      <c r="D101" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E101" s="8" t="s">
-        <v>22</v>
-      </c>
+      <c r="D101" s="8"/>
+      <c r="E101" s="8"/>
       <c r="F101">
         <v>0</v>
       </c>
@@ -3318,14 +3311,8 @@
         <f>VLOOKUP(B102,team!A:B,2,FALSE)</f>
         <v>Raji</v>
       </c>
-      <c r="D102" s="8" t="str">
-        <f>D101</f>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E102" s="8" t="str">
-        <f>E101</f>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D102" s="8"/>
+      <c r="E102" s="8"/>
       <c r="F102">
         <v>0</v>
       </c>
@@ -3345,14 +3332,8 @@
         <f>VLOOKUP(B103,team!A:B,2,FALSE)</f>
         <v>Belle</v>
       </c>
-      <c r="D103" s="8" t="str">
-        <f t="shared" ref="D103:D150" si="1">D102</f>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E103" s="8" t="str">
-        <f t="shared" ref="E103:E150" si="2">E102</f>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D103" s="8"/>
+      <c r="E103" s="8"/>
       <c r="F103">
         <v>0</v>
       </c>
@@ -3372,14 +3353,8 @@
         <f>VLOOKUP(B104,team!A:B,2,FALSE)</f>
         <v>David</v>
       </c>
-      <c r="D104" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E104" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D104" s="8"/>
+      <c r="E104" s="8"/>
       <c r="F104">
         <v>0</v>
       </c>
@@ -3399,14 +3374,8 @@
         <f>VLOOKUP(B105,team!A:B,2,FALSE)</f>
         <v>Shady</v>
       </c>
-      <c r="D105" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E105" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D105" s="8"/>
+      <c r="E105" s="8"/>
       <c r="F105">
         <v>0</v>
       </c>
@@ -3426,14 +3395,8 @@
         <f>VLOOKUP(B106,team!A:B,2,FALSE)</f>
         <v>Shady</v>
       </c>
-      <c r="D106" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E106" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D106" s="8"/>
+      <c r="E106" s="8"/>
       <c r="F106">
         <v>0</v>
       </c>
@@ -3453,14 +3416,8 @@
         <f>VLOOKUP(B107,team!A:B,2,FALSE)</f>
         <v>Kate</v>
       </c>
-      <c r="D107" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E107" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D107" s="8"/>
+      <c r="E107" s="8"/>
       <c r="F107">
         <v>0</v>
       </c>
@@ -3480,14 +3437,8 @@
         <f>VLOOKUP(B108,team!A:B,2,FALSE)</f>
         <v>Raji</v>
       </c>
-      <c r="D108" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E108" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
       <c r="F108">
         <v>0</v>
       </c>
@@ -3507,14 +3458,8 @@
         <f>VLOOKUP(B109,team!A:B,2,FALSE)</f>
         <v>David</v>
       </c>
-      <c r="D109" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E109" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D109" s="8"/>
+      <c r="E109" s="8"/>
       <c r="F109">
         <v>0</v>
       </c>
@@ -3534,14 +3479,8 @@
         <f>VLOOKUP(B110,team!A:B,2,FALSE)</f>
         <v>Belle</v>
       </c>
-      <c r="D110" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E110" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8"/>
       <c r="F110">
         <v>0</v>
       </c>
@@ -3561,14 +3500,8 @@
         <f>VLOOKUP(B111,team!A:B,2,FALSE)</f>
         <v>Brooke</v>
       </c>
-      <c r="D111" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E111" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D111" s="8"/>
+      <c r="E111" s="8"/>
       <c r="F111">
         <v>0</v>
       </c>
@@ -3588,14 +3521,8 @@
         <f>VLOOKUP(B112,team!A:B,2,FALSE)</f>
         <v>Belle</v>
       </c>
-      <c r="D112" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E112" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D112" s="8"/>
+      <c r="E112" s="8"/>
       <c r="F112">
         <v>0</v>
       </c>
@@ -3615,14 +3542,8 @@
         <f>VLOOKUP(B113,team!A:B,2,FALSE)</f>
         <v>David</v>
       </c>
-      <c r="D113" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E113" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D113" s="8"/>
+      <c r="E113" s="8"/>
       <c r="F113">
         <v>0</v>
       </c>
@@ -3642,14 +3563,8 @@
         <f>VLOOKUP(B114,team!A:B,2,FALSE)</f>
         <v>Ben</v>
       </c>
-      <c r="D114" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E114" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D114" s="8"/>
+      <c r="E114" s="8"/>
       <c r="F114">
         <v>0</v>
       </c>
@@ -3669,14 +3584,8 @@
         <f>VLOOKUP(B115,team!A:B,2,FALSE)</f>
         <v>Brooke</v>
       </c>
-      <c r="D115" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E115" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D115" s="8"/>
+      <c r="E115" s="8"/>
       <c r="F115">
         <v>0</v>
       </c>
@@ -3696,14 +3605,8 @@
         <f>VLOOKUP(B116,team!A:B,2,FALSE)</f>
         <v>David</v>
       </c>
-      <c r="D116" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E116" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D116" s="8"/>
+      <c r="E116" s="8"/>
       <c r="F116">
         <v>0</v>
       </c>
@@ -3723,14 +3626,8 @@
         <f>VLOOKUP(B117,team!A:B,2,FALSE)</f>
         <v>Nate</v>
       </c>
-      <c r="D117" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E117" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D117" s="8"/>
+      <c r="E117" s="8"/>
       <c r="F117">
         <v>0</v>
       </c>
@@ -3750,14 +3647,8 @@
         <f>VLOOKUP(B118,team!A:B,2,FALSE)</f>
         <v>Nate</v>
       </c>
-      <c r="D118" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E118" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D118" s="8"/>
+      <c r="E118" s="8"/>
       <c r="F118">
         <v>0</v>
       </c>
@@ -3777,14 +3668,8 @@
         <f>VLOOKUP(B119,team!A:B,2,FALSE)</f>
         <v>Hanson</v>
       </c>
-      <c r="D119" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E119" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D119" s="8"/>
+      <c r="E119" s="8"/>
       <c r="F119">
         <v>0</v>
       </c>
@@ -3804,14 +3689,8 @@
         <f>VLOOKUP(B120,team!A:B,2,FALSE)</f>
         <v>Nate</v>
       </c>
-      <c r="D120" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E120" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D120" s="8"/>
+      <c r="E120" s="8"/>
       <c r="F120">
         <v>0</v>
       </c>
@@ -3831,14 +3710,8 @@
         <f>VLOOKUP(B121,team!A:B,2,FALSE)</f>
         <v>Brooke</v>
       </c>
-      <c r="D121" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E121" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D121" s="8"/>
+      <c r="E121" s="8"/>
       <c r="F121">
         <v>0</v>
       </c>
@@ -3858,14 +3731,8 @@
         <f>VLOOKUP(B122,team!A:B,2,FALSE)</f>
         <v>Raji</v>
       </c>
-      <c r="D122" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E122" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D122" s="8"/>
+      <c r="E122" s="8"/>
       <c r="F122">
         <v>0</v>
       </c>
@@ -3885,14 +3752,8 @@
         <f>VLOOKUP(B123,team!A:B,2,FALSE)</f>
         <v>Hanson</v>
       </c>
-      <c r="D123" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E123" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D123" s="8"/>
+      <c r="E123" s="8"/>
       <c r="F123">
         <v>0</v>
       </c>
@@ -3912,14 +3773,8 @@
         <f>VLOOKUP(B124,team!A:B,2,FALSE)</f>
         <v>Kate</v>
       </c>
-      <c r="D124" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E124" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D124" s="8"/>
+      <c r="E124" s="8"/>
       <c r="F124">
         <v>0</v>
       </c>
@@ -3939,14 +3794,8 @@
         <f>VLOOKUP(B125,team!A:B,2,FALSE)</f>
         <v>Ben</v>
       </c>
-      <c r="D125" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E125" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D125" s="8"/>
+      <c r="E125" s="8"/>
       <c r="F125">
         <v>0</v>
       </c>
@@ -3966,14 +3815,8 @@
         <f>VLOOKUP(B126,team!A:B,2,FALSE)</f>
         <v>Raji</v>
       </c>
-      <c r="D126" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E126" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D126" s="8"/>
+      <c r="E126" s="8"/>
       <c r="F126">
         <v>0</v>
       </c>
@@ -3993,14 +3836,8 @@
         <f>VLOOKUP(B127,team!A:B,2,FALSE)</f>
         <v>Belle</v>
       </c>
-      <c r="D127" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E127" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D127" s="8"/>
+      <c r="E127" s="8"/>
       <c r="F127">
         <v>0</v>
       </c>
@@ -4020,14 +3857,8 @@
         <f>VLOOKUP(B128,team!A:B,2,FALSE)</f>
         <v>Raji</v>
       </c>
-      <c r="D128" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E128" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D128" s="8"/>
+      <c r="E128" s="8"/>
       <c r="F128">
         <v>0</v>
       </c>
@@ -4047,14 +3878,8 @@
         <f>VLOOKUP(B129,team!A:B,2,FALSE)</f>
         <v>Hanson</v>
       </c>
-      <c r="D129" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E129" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D129" s="8"/>
+      <c r="E129" s="8"/>
       <c r="F129">
         <v>0</v>
       </c>
@@ -4074,14 +3899,8 @@
         <f>VLOOKUP(B130,team!A:B,2,FALSE)</f>
         <v>Luigi</v>
       </c>
-      <c r="D130" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E130" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D130" s="8"/>
+      <c r="E130" s="8"/>
       <c r="F130">
         <v>0</v>
       </c>
@@ -4101,14 +3920,8 @@
         <f>VLOOKUP(B131,team!A:B,2,FALSE)</f>
         <v>Brooke</v>
       </c>
-      <c r="D131" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E131" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D131" s="8"/>
+      <c r="E131" s="8"/>
       <c r="F131">
         <v>0</v>
       </c>
@@ -4128,14 +3941,8 @@
         <f>VLOOKUP(B132,team!A:B,2,FALSE)</f>
         <v>Belle</v>
       </c>
-      <c r="D132" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E132" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D132" s="8"/>
+      <c r="E132" s="8"/>
       <c r="F132">
         <v>0</v>
       </c>
@@ -4155,14 +3962,8 @@
         <f>VLOOKUP(B133,team!A:B,2,FALSE)</f>
         <v>Ben</v>
       </c>
-      <c r="D133" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E133" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D133" s="8"/>
+      <c r="E133" s="8"/>
       <c r="F133">
         <v>0</v>
       </c>
@@ -4182,14 +3983,8 @@
         <f>VLOOKUP(B134,team!A:B,2,FALSE)</f>
         <v>Luigi</v>
       </c>
-      <c r="D134" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E134" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D134" s="8"/>
+      <c r="E134" s="8"/>
       <c r="F134">
         <v>0</v>
       </c>
@@ -4209,14 +4004,8 @@
         <f>VLOOKUP(B135,team!A:B,2,FALSE)</f>
         <v>David</v>
       </c>
-      <c r="D135" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E135" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D135" s="8"/>
+      <c r="E135" s="8"/>
       <c r="F135">
         <v>0</v>
       </c>
@@ -4236,14 +4025,8 @@
         <f>VLOOKUP(B136,team!A:B,2,FALSE)</f>
         <v>David</v>
       </c>
-      <c r="D136" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E136" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D136" s="8"/>
+      <c r="E136" s="8"/>
       <c r="F136">
         <v>0</v>
       </c>
@@ -4263,14 +4046,8 @@
         <f>VLOOKUP(B137,team!A:B,2,FALSE)</f>
         <v>Hanson</v>
       </c>
-      <c r="D137" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E137" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D137" s="8"/>
+      <c r="E137" s="8"/>
       <c r="F137">
         <v>0</v>
       </c>
@@ -4290,14 +4067,8 @@
         <f>VLOOKUP(B138,team!A:B,2,FALSE)</f>
         <v>David</v>
       </c>
-      <c r="D138" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E138" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D138" s="8"/>
+      <c r="E138" s="8"/>
       <c r="F138">
         <v>0</v>
       </c>
@@ -4317,14 +4088,8 @@
         <f>VLOOKUP(B139,team!A:B,2,FALSE)</f>
         <v>Hanson</v>
       </c>
-      <c r="D139" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E139" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D139" s="8"/>
+      <c r="E139" s="8"/>
       <c r="F139">
         <v>0</v>
       </c>
@@ -4344,14 +4109,8 @@
         <f>VLOOKUP(B140,team!A:B,2,FALSE)</f>
         <v>Raji</v>
       </c>
-      <c r="D140" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E140" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D140" s="8"/>
+      <c r="E140" s="8"/>
       <c r="F140">
         <v>0</v>
       </c>
@@ -4371,14 +4130,8 @@
         <f>VLOOKUP(B141,team!A:B,2,FALSE)</f>
         <v>Luigi</v>
       </c>
-      <c r="D141" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E141" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D141" s="8"/>
+      <c r="E141" s="8"/>
       <c r="F141">
         <v>0</v>
       </c>
@@ -4398,14 +4151,8 @@
         <f>VLOOKUP(B142,team!A:B,2,FALSE)</f>
         <v>Raji</v>
       </c>
-      <c r="D142" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E142" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D142" s="8"/>
+      <c r="E142" s="8"/>
       <c r="F142">
         <v>0</v>
       </c>
@@ -4425,14 +4172,8 @@
         <f>VLOOKUP(B143,team!A:B,2,FALSE)</f>
         <v>Hanson</v>
       </c>
-      <c r="D143" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E143" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D143" s="8"/>
+      <c r="E143" s="8"/>
       <c r="F143">
         <v>0</v>
       </c>
@@ -4452,14 +4193,8 @@
         <f>VLOOKUP(B144,team!A:B,2,FALSE)</f>
         <v>Belle</v>
       </c>
-      <c r="D144" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E144" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D144" s="8"/>
+      <c r="E144" s="8"/>
       <c r="F144">
         <v>0</v>
       </c>
@@ -4479,14 +4214,8 @@
         <f>VLOOKUP(B145,team!A:B,2,FALSE)</f>
         <v>Shady</v>
       </c>
-      <c r="D145" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E145" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D145" s="8"/>
+      <c r="E145" s="8"/>
       <c r="F145">
         <v>0</v>
       </c>
@@ -4506,14 +4235,8 @@
         <f>VLOOKUP(B146,team!A:B,2,FALSE)</f>
         <v>Raji</v>
       </c>
-      <c r="D146" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E146" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D146" s="8"/>
+      <c r="E146" s="8"/>
       <c r="F146">
         <v>0</v>
       </c>
@@ -4533,14 +4256,8 @@
         <f>VLOOKUP(B147,team!A:B,2,FALSE)</f>
         <v>Kate</v>
       </c>
-      <c r="D147" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E147" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D147" s="8"/>
+      <c r="E147" s="8"/>
       <c r="F147">
         <v>0</v>
       </c>
@@ -4560,14 +4277,8 @@
         <f>VLOOKUP(B148,team!A:B,2,FALSE)</f>
         <v>Nate</v>
       </c>
-      <c r="D148" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E148" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D148" s="8"/>
+      <c r="E148" s="8"/>
       <c r="F148">
         <v>0</v>
       </c>
@@ -4587,14 +4298,8 @@
         <f>VLOOKUP(B149,team!A:B,2,FALSE)</f>
         <v>Hanson</v>
       </c>
-      <c r="D149" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E149" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D149" s="8"/>
+      <c r="E149" s="8"/>
       <c r="F149">
         <v>0</v>
       </c>
@@ -4614,14 +4319,8 @@
         <f>VLOOKUP(B150,team!A:B,2,FALSE)</f>
         <v>Brooke</v>
       </c>
-      <c r="D150" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>0/0/0000</v>
-      </c>
-      <c r="E150" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>0/0/0000</v>
-      </c>
+      <c r="D150" s="8"/>
+      <c r="E150" s="8"/>
       <c r="F150">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Updated db.oy file date import issue
</commit_message>
<xml_diff>
--- a/backend/data.xlsx
+++ b/backend/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raji Roy\Desktop\CRM Project\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DC465D-8CBF-4D12-A822-66DBCE2C0A87}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8569F4BF-4937-4ED3-9C34-A7B8EB4C11AA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -964,7 +964,7 @@
   <dimension ref="A1:G150"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101:E150"/>
+      <selection activeCell="E84" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3290,8 +3290,12 @@
         <f>VLOOKUP(B101,team!A:B,2,FALSE)</f>
         <v>Belle</v>
       </c>
-      <c r="D101" s="8"/>
-      <c r="E101" s="8"/>
+      <c r="D101" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E101" s="8">
+        <v>21916</v>
+      </c>
       <c r="F101">
         <v>0</v>
       </c>
@@ -3311,8 +3315,12 @@
         <f>VLOOKUP(B102,team!A:B,2,FALSE)</f>
         <v>Raji</v>
       </c>
-      <c r="D102" s="8"/>
-      <c r="E102" s="8"/>
+      <c r="D102" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E102" s="8">
+        <v>21916</v>
+      </c>
       <c r="F102">
         <v>0</v>
       </c>
@@ -3332,8 +3340,12 @@
         <f>VLOOKUP(B103,team!A:B,2,FALSE)</f>
         <v>Belle</v>
       </c>
-      <c r="D103" s="8"/>
-      <c r="E103" s="8"/>
+      <c r="D103" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E103" s="8">
+        <v>21916</v>
+      </c>
       <c r="F103">
         <v>0</v>
       </c>
@@ -3353,8 +3365,12 @@
         <f>VLOOKUP(B104,team!A:B,2,FALSE)</f>
         <v>David</v>
       </c>
-      <c r="D104" s="8"/>
-      <c r="E104" s="8"/>
+      <c r="D104" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E104" s="8">
+        <v>21916</v>
+      </c>
       <c r="F104">
         <v>0</v>
       </c>
@@ -3374,8 +3390,12 @@
         <f>VLOOKUP(B105,team!A:B,2,FALSE)</f>
         <v>Shady</v>
       </c>
-      <c r="D105" s="8"/>
-      <c r="E105" s="8"/>
+      <c r="D105" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E105" s="8">
+        <v>21916</v>
+      </c>
       <c r="F105">
         <v>0</v>
       </c>
@@ -3395,8 +3415,12 @@
         <f>VLOOKUP(B106,team!A:B,2,FALSE)</f>
         <v>Shady</v>
       </c>
-      <c r="D106" s="8"/>
-      <c r="E106" s="8"/>
+      <c r="D106" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E106" s="8">
+        <v>21916</v>
+      </c>
       <c r="F106">
         <v>0</v>
       </c>
@@ -3416,8 +3440,12 @@
         <f>VLOOKUP(B107,team!A:B,2,FALSE)</f>
         <v>Kate</v>
       </c>
-      <c r="D107" s="8"/>
-      <c r="E107" s="8"/>
+      <c r="D107" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E107" s="8">
+        <v>21916</v>
+      </c>
       <c r="F107">
         <v>0</v>
       </c>
@@ -3437,8 +3465,12 @@
         <f>VLOOKUP(B108,team!A:B,2,FALSE)</f>
         <v>Raji</v>
       </c>
-      <c r="D108" s="8"/>
-      <c r="E108" s="8"/>
+      <c r="D108" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E108" s="8">
+        <v>21916</v>
+      </c>
       <c r="F108">
         <v>0</v>
       </c>
@@ -3458,8 +3490,12 @@
         <f>VLOOKUP(B109,team!A:B,2,FALSE)</f>
         <v>David</v>
       </c>
-      <c r="D109" s="8"/>
-      <c r="E109" s="8"/>
+      <c r="D109" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E109" s="8">
+        <v>21916</v>
+      </c>
       <c r="F109">
         <v>0</v>
       </c>
@@ -3479,8 +3515,12 @@
         <f>VLOOKUP(B110,team!A:B,2,FALSE)</f>
         <v>Belle</v>
       </c>
-      <c r="D110" s="8"/>
-      <c r="E110" s="8"/>
+      <c r="D110" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E110" s="8">
+        <v>21916</v>
+      </c>
       <c r="F110">
         <v>0</v>
       </c>
@@ -3500,8 +3540,12 @@
         <f>VLOOKUP(B111,team!A:B,2,FALSE)</f>
         <v>Brooke</v>
       </c>
-      <c r="D111" s="8"/>
-      <c r="E111" s="8"/>
+      <c r="D111" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E111" s="8">
+        <v>21916</v>
+      </c>
       <c r="F111">
         <v>0</v>
       </c>
@@ -3521,8 +3565,12 @@
         <f>VLOOKUP(B112,team!A:B,2,FALSE)</f>
         <v>Belle</v>
       </c>
-      <c r="D112" s="8"/>
-      <c r="E112" s="8"/>
+      <c r="D112" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E112" s="8">
+        <v>21916</v>
+      </c>
       <c r="F112">
         <v>0</v>
       </c>
@@ -3542,8 +3590,12 @@
         <f>VLOOKUP(B113,team!A:B,2,FALSE)</f>
         <v>David</v>
       </c>
-      <c r="D113" s="8"/>
-      <c r="E113" s="8"/>
+      <c r="D113" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E113" s="8">
+        <v>21916</v>
+      </c>
       <c r="F113">
         <v>0</v>
       </c>
@@ -3563,8 +3615,12 @@
         <f>VLOOKUP(B114,team!A:B,2,FALSE)</f>
         <v>Ben</v>
       </c>
-      <c r="D114" s="8"/>
-      <c r="E114" s="8"/>
+      <c r="D114" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E114" s="8">
+        <v>21916</v>
+      </c>
       <c r="F114">
         <v>0</v>
       </c>
@@ -3584,8 +3640,12 @@
         <f>VLOOKUP(B115,team!A:B,2,FALSE)</f>
         <v>Brooke</v>
       </c>
-      <c r="D115" s="8"/>
-      <c r="E115" s="8"/>
+      <c r="D115" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E115" s="8">
+        <v>21916</v>
+      </c>
       <c r="F115">
         <v>0</v>
       </c>
@@ -3605,8 +3665,12 @@
         <f>VLOOKUP(B116,team!A:B,2,FALSE)</f>
         <v>David</v>
       </c>
-      <c r="D116" s="8"/>
-      <c r="E116" s="8"/>
+      <c r="D116" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E116" s="8">
+        <v>21916</v>
+      </c>
       <c r="F116">
         <v>0</v>
       </c>
@@ -3626,8 +3690,12 @@
         <f>VLOOKUP(B117,team!A:B,2,FALSE)</f>
         <v>Nate</v>
       </c>
-      <c r="D117" s="8"/>
-      <c r="E117" s="8"/>
+      <c r="D117" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E117" s="8">
+        <v>21916</v>
+      </c>
       <c r="F117">
         <v>0</v>
       </c>
@@ -3647,8 +3715,12 @@
         <f>VLOOKUP(B118,team!A:B,2,FALSE)</f>
         <v>Nate</v>
       </c>
-      <c r="D118" s="8"/>
-      <c r="E118" s="8"/>
+      <c r="D118" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E118" s="8">
+        <v>21916</v>
+      </c>
       <c r="F118">
         <v>0</v>
       </c>
@@ -3668,8 +3740,12 @@
         <f>VLOOKUP(B119,team!A:B,2,FALSE)</f>
         <v>Hanson</v>
       </c>
-      <c r="D119" s="8"/>
-      <c r="E119" s="8"/>
+      <c r="D119" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E119" s="8">
+        <v>21916</v>
+      </c>
       <c r="F119">
         <v>0</v>
       </c>
@@ -3689,8 +3765,12 @@
         <f>VLOOKUP(B120,team!A:B,2,FALSE)</f>
         <v>Nate</v>
       </c>
-      <c r="D120" s="8"/>
-      <c r="E120" s="8"/>
+      <c r="D120" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E120" s="8">
+        <v>21916</v>
+      </c>
       <c r="F120">
         <v>0</v>
       </c>
@@ -3710,8 +3790,12 @@
         <f>VLOOKUP(B121,team!A:B,2,FALSE)</f>
         <v>Brooke</v>
       </c>
-      <c r="D121" s="8"/>
-      <c r="E121" s="8"/>
+      <c r="D121" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E121" s="8">
+        <v>21916</v>
+      </c>
       <c r="F121">
         <v>0</v>
       </c>
@@ -3731,8 +3815,12 @@
         <f>VLOOKUP(B122,team!A:B,2,FALSE)</f>
         <v>Raji</v>
       </c>
-      <c r="D122" s="8"/>
-      <c r="E122" s="8"/>
+      <c r="D122" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E122" s="8">
+        <v>21916</v>
+      </c>
       <c r="F122">
         <v>0</v>
       </c>
@@ -3752,8 +3840,12 @@
         <f>VLOOKUP(B123,team!A:B,2,FALSE)</f>
         <v>Hanson</v>
       </c>
-      <c r="D123" s="8"/>
-      <c r="E123" s="8"/>
+      <c r="D123" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E123" s="8">
+        <v>21916</v>
+      </c>
       <c r="F123">
         <v>0</v>
       </c>
@@ -3773,8 +3865,12 @@
         <f>VLOOKUP(B124,team!A:B,2,FALSE)</f>
         <v>Kate</v>
       </c>
-      <c r="D124" s="8"/>
-      <c r="E124" s="8"/>
+      <c r="D124" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E124" s="8">
+        <v>21916</v>
+      </c>
       <c r="F124">
         <v>0</v>
       </c>
@@ -3794,8 +3890,12 @@
         <f>VLOOKUP(B125,team!A:B,2,FALSE)</f>
         <v>Ben</v>
       </c>
-      <c r="D125" s="8"/>
-      <c r="E125" s="8"/>
+      <c r="D125" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E125" s="8">
+        <v>21916</v>
+      </c>
       <c r="F125">
         <v>0</v>
       </c>
@@ -3815,8 +3915,12 @@
         <f>VLOOKUP(B126,team!A:B,2,FALSE)</f>
         <v>Raji</v>
       </c>
-      <c r="D126" s="8"/>
-      <c r="E126" s="8"/>
+      <c r="D126" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E126" s="8">
+        <v>21916</v>
+      </c>
       <c r="F126">
         <v>0</v>
       </c>
@@ -3836,8 +3940,12 @@
         <f>VLOOKUP(B127,team!A:B,2,FALSE)</f>
         <v>Belle</v>
       </c>
-      <c r="D127" s="8"/>
-      <c r="E127" s="8"/>
+      <c r="D127" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E127" s="8">
+        <v>21916</v>
+      </c>
       <c r="F127">
         <v>0</v>
       </c>
@@ -3857,8 +3965,12 @@
         <f>VLOOKUP(B128,team!A:B,2,FALSE)</f>
         <v>Raji</v>
       </c>
-      <c r="D128" s="8"/>
-      <c r="E128" s="8"/>
+      <c r="D128" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E128" s="8">
+        <v>21916</v>
+      </c>
       <c r="F128">
         <v>0</v>
       </c>
@@ -3878,8 +3990,12 @@
         <f>VLOOKUP(B129,team!A:B,2,FALSE)</f>
         <v>Hanson</v>
       </c>
-      <c r="D129" s="8"/>
-      <c r="E129" s="8"/>
+      <c r="D129" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E129" s="8">
+        <v>21916</v>
+      </c>
       <c r="F129">
         <v>0</v>
       </c>
@@ -3899,8 +4015,12 @@
         <f>VLOOKUP(B130,team!A:B,2,FALSE)</f>
         <v>Luigi</v>
       </c>
-      <c r="D130" s="8"/>
-      <c r="E130" s="8"/>
+      <c r="D130" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E130" s="8">
+        <v>21916</v>
+      </c>
       <c r="F130">
         <v>0</v>
       </c>
@@ -3920,8 +4040,12 @@
         <f>VLOOKUP(B131,team!A:B,2,FALSE)</f>
         <v>Brooke</v>
       </c>
-      <c r="D131" s="8"/>
-      <c r="E131" s="8"/>
+      <c r="D131" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E131" s="8">
+        <v>21916</v>
+      </c>
       <c r="F131">
         <v>0</v>
       </c>
@@ -3941,8 +4065,12 @@
         <f>VLOOKUP(B132,team!A:B,2,FALSE)</f>
         <v>Belle</v>
       </c>
-      <c r="D132" s="8"/>
-      <c r="E132" s="8"/>
+      <c r="D132" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E132" s="8">
+        <v>21916</v>
+      </c>
       <c r="F132">
         <v>0</v>
       </c>
@@ -3962,8 +4090,12 @@
         <f>VLOOKUP(B133,team!A:B,2,FALSE)</f>
         <v>Ben</v>
       </c>
-      <c r="D133" s="8"/>
-      <c r="E133" s="8"/>
+      <c r="D133" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E133" s="8">
+        <v>21916</v>
+      </c>
       <c r="F133">
         <v>0</v>
       </c>
@@ -3983,8 +4115,12 @@
         <f>VLOOKUP(B134,team!A:B,2,FALSE)</f>
         <v>Luigi</v>
       </c>
-      <c r="D134" s="8"/>
-      <c r="E134" s="8"/>
+      <c r="D134" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E134" s="8">
+        <v>21916</v>
+      </c>
       <c r="F134">
         <v>0</v>
       </c>
@@ -4004,8 +4140,12 @@
         <f>VLOOKUP(B135,team!A:B,2,FALSE)</f>
         <v>David</v>
       </c>
-      <c r="D135" s="8"/>
-      <c r="E135" s="8"/>
+      <c r="D135" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E135" s="8">
+        <v>21916</v>
+      </c>
       <c r="F135">
         <v>0</v>
       </c>
@@ -4025,8 +4165,12 @@
         <f>VLOOKUP(B136,team!A:B,2,FALSE)</f>
         <v>David</v>
       </c>
-      <c r="D136" s="8"/>
-      <c r="E136" s="8"/>
+      <c r="D136" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E136" s="8">
+        <v>21916</v>
+      </c>
       <c r="F136">
         <v>0</v>
       </c>
@@ -4046,8 +4190,12 @@
         <f>VLOOKUP(B137,team!A:B,2,FALSE)</f>
         <v>Hanson</v>
       </c>
-      <c r="D137" s="8"/>
-      <c r="E137" s="8"/>
+      <c r="D137" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E137" s="8">
+        <v>21916</v>
+      </c>
       <c r="F137">
         <v>0</v>
       </c>
@@ -4067,8 +4215,12 @@
         <f>VLOOKUP(B138,team!A:B,2,FALSE)</f>
         <v>David</v>
       </c>
-      <c r="D138" s="8"/>
-      <c r="E138" s="8"/>
+      <c r="D138" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E138" s="8">
+        <v>21916</v>
+      </c>
       <c r="F138">
         <v>0</v>
       </c>
@@ -4088,8 +4240,12 @@
         <f>VLOOKUP(B139,team!A:B,2,FALSE)</f>
         <v>Hanson</v>
       </c>
-      <c r="D139" s="8"/>
-      <c r="E139" s="8"/>
+      <c r="D139" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E139" s="8">
+        <v>21916</v>
+      </c>
       <c r="F139">
         <v>0</v>
       </c>
@@ -4109,8 +4265,12 @@
         <f>VLOOKUP(B140,team!A:B,2,FALSE)</f>
         <v>Raji</v>
       </c>
-      <c r="D140" s="8"/>
-      <c r="E140" s="8"/>
+      <c r="D140" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E140" s="8">
+        <v>21916</v>
+      </c>
       <c r="F140">
         <v>0</v>
       </c>
@@ -4130,8 +4290,12 @@
         <f>VLOOKUP(B141,team!A:B,2,FALSE)</f>
         <v>Luigi</v>
       </c>
-      <c r="D141" s="8"/>
-      <c r="E141" s="8"/>
+      <c r="D141" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E141" s="8">
+        <v>21916</v>
+      </c>
       <c r="F141">
         <v>0</v>
       </c>
@@ -4151,8 +4315,12 @@
         <f>VLOOKUP(B142,team!A:B,2,FALSE)</f>
         <v>Raji</v>
       </c>
-      <c r="D142" s="8"/>
-      <c r="E142" s="8"/>
+      <c r="D142" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E142" s="8">
+        <v>21916</v>
+      </c>
       <c r="F142">
         <v>0</v>
       </c>
@@ -4172,8 +4340,12 @@
         <f>VLOOKUP(B143,team!A:B,2,FALSE)</f>
         <v>Hanson</v>
       </c>
-      <c r="D143" s="8"/>
-      <c r="E143" s="8"/>
+      <c r="D143" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E143" s="8">
+        <v>21916</v>
+      </c>
       <c r="F143">
         <v>0</v>
       </c>
@@ -4193,8 +4365,12 @@
         <f>VLOOKUP(B144,team!A:B,2,FALSE)</f>
         <v>Belle</v>
       </c>
-      <c r="D144" s="8"/>
-      <c r="E144" s="8"/>
+      <c r="D144" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E144" s="8">
+        <v>21916</v>
+      </c>
       <c r="F144">
         <v>0</v>
       </c>
@@ -4214,8 +4390,12 @@
         <f>VLOOKUP(B145,team!A:B,2,FALSE)</f>
         <v>Shady</v>
       </c>
-      <c r="D145" s="8"/>
-      <c r="E145" s="8"/>
+      <c r="D145" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E145" s="8">
+        <v>21916</v>
+      </c>
       <c r="F145">
         <v>0</v>
       </c>
@@ -4235,8 +4415,12 @@
         <f>VLOOKUP(B146,team!A:B,2,FALSE)</f>
         <v>Raji</v>
       </c>
-      <c r="D146" s="8"/>
-      <c r="E146" s="8"/>
+      <c r="D146" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E146" s="8">
+        <v>21916</v>
+      </c>
       <c r="F146">
         <v>0</v>
       </c>
@@ -4256,8 +4440,12 @@
         <f>VLOOKUP(B147,team!A:B,2,FALSE)</f>
         <v>Kate</v>
       </c>
-      <c r="D147" s="8"/>
-      <c r="E147" s="8"/>
+      <c r="D147" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E147" s="8">
+        <v>21916</v>
+      </c>
       <c r="F147">
         <v>0</v>
       </c>
@@ -4277,8 +4465,12 @@
         <f>VLOOKUP(B148,team!A:B,2,FALSE)</f>
         <v>Nate</v>
       </c>
-      <c r="D148" s="8"/>
-      <c r="E148" s="8"/>
+      <c r="D148" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E148" s="8">
+        <v>21916</v>
+      </c>
       <c r="F148">
         <v>0</v>
       </c>
@@ -4298,8 +4490,12 @@
         <f>VLOOKUP(B149,team!A:B,2,FALSE)</f>
         <v>Hanson</v>
       </c>
-      <c r="D149" s="8"/>
-      <c r="E149" s="8"/>
+      <c r="D149" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E149" s="8">
+        <v>21916</v>
+      </c>
       <c r="F149">
         <v>0</v>
       </c>
@@ -4319,8 +4515,12 @@
         <f>VLOOKUP(B150,team!A:B,2,FALSE)</f>
         <v>Brooke</v>
       </c>
-      <c r="D150" s="8"/>
-      <c r="E150" s="8"/>
+      <c r="D150" s="8">
+        <v>21916</v>
+      </c>
+      <c r="E150" s="8">
+        <v>21916</v>
+      </c>
       <c r="F150">
         <v>0</v>
       </c>

</xml_diff>